<commit_message>
edits following manuscript reviews
</commit_message>
<xml_diff>
--- a/source_data/Settlement-stage larvae.xlsx
+++ b/source_data/Settlement-stage larvae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rworking_projects\tropical_ucrit_data\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E00B602-88F7-47E4-894D-393765CF0C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003B8D31-0250-4209-856D-8A7FC6456468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="2475" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4050" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Moorea" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2169" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="484">
   <si>
     <t>fish ID</t>
   </si>
@@ -1425,6 +1425,54 @@
   </si>
   <si>
     <t>2 fish in lane 5</t>
+  </si>
+  <si>
+    <t>JML1</t>
+  </si>
+  <si>
+    <t>JML2</t>
+  </si>
+  <si>
+    <t>JML3</t>
+  </si>
+  <si>
+    <t>JML4</t>
+  </si>
+  <si>
+    <t>JML5</t>
+  </si>
+  <si>
+    <t>JML6</t>
+  </si>
+  <si>
+    <t>JML7</t>
+  </si>
+  <si>
+    <t>JML8</t>
+  </si>
+  <si>
+    <t>JML9</t>
+  </si>
+  <si>
+    <t>JML10</t>
+  </si>
+  <si>
+    <t>JML11</t>
+  </si>
+  <si>
+    <t>JML12</t>
+  </si>
+  <si>
+    <t>JML13</t>
+  </si>
+  <si>
+    <t>JML14</t>
+  </si>
+  <si>
+    <t>JML15</t>
+  </si>
+  <si>
+    <t>JML16</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1482,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1616,6 +1664,12 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2484,9 +2538,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R49" sqref="R49"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2495,7 +2549,9 @@
     <col min="3" max="3" width="8.28515625" style="48"/>
     <col min="4" max="6" width="8.28515625" style="19"/>
     <col min="7" max="8" width="8.28515625" style="46"/>
-    <col min="9" max="11" width="8.28515625" style="19"/>
+    <col min="9" max="9" width="8.28515625" style="19"/>
+    <col min="10" max="10" width="13.85546875" style="19" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="19"/>
     <col min="12" max="13" width="8.28515625" style="52"/>
     <col min="14" max="15" width="8.28515625" style="19"/>
     <col min="16" max="16" width="8.28515625" style="51"/>
@@ -11232,7 +11288,9 @@
       <c r="I138" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J138" s="60"/>
+      <c r="J138" s="60" t="s">
+        <v>468</v>
+      </c>
       <c r="K138" s="40" t="s">
         <v>17</v>
       </c>
@@ -11292,7 +11350,9 @@
       <c r="I139" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J139" s="60"/>
+      <c r="J139" s="60" t="s">
+        <v>469</v>
+      </c>
       <c r="K139" s="40" t="s">
         <v>176</v>
       </c>
@@ -11352,7 +11412,9 @@
       <c r="I140" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J140" s="60"/>
+      <c r="J140" s="60" t="s">
+        <v>470</v>
+      </c>
       <c r="K140" s="40" t="s">
         <v>18</v>
       </c>
@@ -11412,7 +11474,9 @@
       <c r="I141" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J141" s="63"/>
+      <c r="J141" s="60" t="s">
+        <v>471</v>
+      </c>
       <c r="K141" s="41" t="s">
         <v>17</v>
       </c>
@@ -11473,7 +11537,9 @@
       <c r="I142" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J142" s="63"/>
+      <c r="J142" s="60" t="s">
+        <v>472</v>
+      </c>
       <c r="K142" s="41" t="s">
         <v>17</v>
       </c>
@@ -11534,7 +11600,9 @@
       <c r="I143" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J143" s="63"/>
+      <c r="J143" s="60" t="s">
+        <v>473</v>
+      </c>
       <c r="K143" s="41" t="s">
         <v>17</v>
       </c>
@@ -11595,7 +11663,9 @@
       <c r="I144" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J144" s="63"/>
+      <c r="J144" s="60" t="s">
+        <v>474</v>
+      </c>
       <c r="K144" s="41" t="s">
         <v>17</v>
       </c>
@@ -11656,7 +11726,9 @@
       <c r="I145" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J145" s="60"/>
+      <c r="J145" s="60" t="s">
+        <v>475</v>
+      </c>
       <c r="K145" s="40" t="s">
         <v>17</v>
       </c>
@@ -11717,7 +11789,9 @@
       <c r="I146" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J146" s="60"/>
+      <c r="J146" s="60" t="s">
+        <v>476</v>
+      </c>
       <c r="K146" s="40" t="s">
         <v>176</v>
       </c>
@@ -11777,7 +11851,9 @@
       <c r="I147" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J147" s="60"/>
+      <c r="J147" s="60" t="s">
+        <v>477</v>
+      </c>
       <c r="K147" s="40" t="s">
         <v>176</v>
       </c>
@@ -11837,7 +11913,9 @@
       <c r="I148" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J148" s="60"/>
+      <c r="J148" s="60" t="s">
+        <v>478</v>
+      </c>
       <c r="K148" s="40" t="s">
         <v>176</v>
       </c>
@@ -11897,7 +11975,9 @@
       <c r="I149" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J149" s="60"/>
+      <c r="J149" s="60" t="s">
+        <v>479</v>
+      </c>
       <c r="K149" s="40" t="s">
         <v>176</v>
       </c>
@@ -11957,7 +12037,9 @@
       <c r="I150" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J150" s="60"/>
+      <c r="J150" s="60" t="s">
+        <v>480</v>
+      </c>
       <c r="K150" s="40" t="s">
         <v>18</v>
       </c>
@@ -12017,7 +12099,9 @@
       <c r="I151" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J151" s="60"/>
+      <c r="J151" s="60" t="s">
+        <v>481</v>
+      </c>
       <c r="K151" s="40" t="s">
         <v>18</v>
       </c>
@@ -12077,7 +12161,9 @@
       <c r="I152" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J152" s="60"/>
+      <c r="J152" s="60" t="s">
+        <v>482</v>
+      </c>
       <c r="K152" s="40" t="s">
         <v>18</v>
       </c>
@@ -12137,7 +12223,9 @@
       <c r="I153" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="J153" s="60"/>
+      <c r="J153" s="60" t="s">
+        <v>483</v>
+      </c>
       <c r="K153" s="40" t="s">
         <v>18</v>
       </c>
@@ -12170,6 +12258,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y55:AB152">
     <sortCondition ref="Y54"/>
   </sortState>
+  <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>